<commit_message>
Pushing the final copy of refactored code
</commit_message>
<xml_diff>
--- a/src/main/java/com/codingRound/testdata/Controller.xlsx
+++ b/src/main/java/com/codingRound/testdata/Controller.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606F11EA-787E-4644-A405-DF74927311E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC898343-36B1-41FB-85B8-F9A0DA621EA7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11280" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
     <sheet name="FlightBookingPage" sheetId="2" r:id="rId2"/>
     <sheet name="HotelBookingPage" sheetId="3" r:id="rId3"/>
+    <sheet name="SignInPage" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -69,6 +70,39 @@
   </si>
   <si>
     <t>HotelBookingTest</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>expectedMessage</t>
+  </si>
+  <si>
+    <t>There were errors in your submission
+Your username is a required field
+Your account password is a required field</t>
+  </si>
+  <si>
+    <t>emptyfields</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>There were errors in your submission
+Your username should be a valid email address.</t>
+  </si>
+  <si>
+    <t>test123</t>
   </si>
 </sst>
 </file>
@@ -125,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -142,6 +176,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -492,7 +530,7 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <f ca="1">TODAY()</f>
-        <v>43607</v>
+        <v>43608</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -540,4 +578,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92C9C00-0B16-4F23-B027-AE51C7D4383A}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>